<commit_message>
làm xong lương mỹ tho
</commit_message>
<xml_diff>
--- a/01.VietSoftHRM/VietSoftHRM/bin/Debug/Template/TemplatePhieuLuongQC.xlsx
+++ b/01.VietSoftHRM/VietSoftHRM/bin/Debug/Template/TemplatePhieuLuongQC.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\HRM_Last\01.VS_HRM\01.VietSoftHRM\VietSoftHRM\bin\Debug\lib\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01.SourceCode\02.HRM\01.VietSoftHRM\VietSoftHRM\bin\Debug\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DF1D2F-1BCE-4A24-B929-A681D29D2FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="18195" windowHeight="11760"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QCChuyen" sheetId="1" r:id="rId1"/>
@@ -23,17 +24,30 @@
     <definedName name="PhieuNhanLuong">QCChuyen!$A$7:$AL$7</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">PhieuLuongQC!$A$1:$E$56</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>User</author>
   </authors>
   <commentList>
-    <comment ref="B37" authorId="0" shapeId="0">
+    <comment ref="B37" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -57,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E37" authorId="0" shapeId="0">
+    <comment ref="E37" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -81,7 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B47" authorId="0" shapeId="0">
+    <comment ref="B47" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -96,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E47" authorId="0" shapeId="0">
+    <comment ref="E47" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -493,14 +507,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,###"/>
     <numFmt numFmtId="165" formatCode="#,###.0;\(#,###.0\);\ ;\ "/>
     <numFmt numFmtId="166" formatCode="#,###;\(#,###\);\ ;\ "/>
     <numFmt numFmtId="167" formatCode="#,##0.0_);\(#,##0.0\)"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="27">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -712,9 +726,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -729,7 +743,7 @@
     <xf numFmtId="166" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -740,21 +754,21 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="37" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="37" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -763,19 +777,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="37" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -783,18 +794,18 @@
     <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="37" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="37" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="37" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -805,6 +816,9 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -819,13 +833,10 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Salary sheets" xfId="1"/>
+    <cellStyle name="Normal_Salary sheets" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -857,7 +868,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1040" name="Line 11"/>
+        <xdr:cNvPr id="1040" name="Line 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
@@ -894,7 +911,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="DSNV"/>
@@ -3296,9 +3313,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3336,9 +3353,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3373,7 +3390,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3408,7 +3425,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3581,17 +3598,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="11" ySplit="5" topLeftCell="L6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="P15" sqref="P15"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="3" max="3" width="21.140625" customWidth="1"/>
@@ -3609,53 +3626,53 @@
     <col min="31" max="35" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" ht="14.25">
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:38" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" ht="14.25">
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:38" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="54" t="s">
+    <row r="3" spans="1:38" ht="25.5">
+      <c r="A3" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="54"/>
-      <c r="S3" s="54"/>
-      <c r="T3" s="54"/>
-      <c r="U3" s="54"/>
-      <c r="V3" s="54"/>
-      <c r="W3" s="54"/>
-      <c r="X3" s="54"/>
-      <c r="Y3" s="54"/>
-      <c r="Z3" s="54"/>
-      <c r="AA3" s="54"/>
-      <c r="AB3" s="54"/>
-      <c r="AC3" s="54"/>
-      <c r="AD3" s="54"/>
-      <c r="AE3" s="54"/>
-      <c r="AF3" s="54"/>
-      <c r="AG3" s="54"/>
-      <c r="AH3" s="54"/>
-      <c r="AI3" s="54"/>
-      <c r="AJ3" s="54"/>
-    </row>
-    <row r="5" spans="1:38" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="48"/>
+      <c r="U3" s="48"/>
+      <c r="V3" s="48"/>
+      <c r="W3" s="48"/>
+      <c r="X3" s="48"/>
+      <c r="Y3" s="48"/>
+      <c r="Z3" s="48"/>
+      <c r="AA3" s="48"/>
+      <c r="AB3" s="48"/>
+      <c r="AC3" s="48"/>
+      <c r="AD3" s="48"/>
+      <c r="AE3" s="48"/>
+      <c r="AF3" s="48"/>
+      <c r="AG3" s="48"/>
+      <c r="AH3" s="48"/>
+      <c r="AI3" s="48"/>
+      <c r="AJ3" s="48"/>
+    </row>
+    <row r="5" spans="1:38" ht="42.75">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -3771,7 +3788,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:38" ht="14.25">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -3887,20 +3904,20 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:38" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" ht="33.75">
       <c r="A7" s="4" t="s">
         <v>85</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="47" t="s">
         <v>89</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -4003,7 +4020,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:38">
       <c r="A8" s="49" t="s">
         <v>36</v>
       </c>
@@ -4151,14 +4168,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="55.85546875" customWidth="1"/>
     <col min="2" max="2" width="27.85546875" customWidth="1"/>
@@ -4167,7 +4184,7 @@
     <col min="5" max="5" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="12.75" customHeight="1">
       <c r="A1" s="12"/>
       <c r="B1" s="13">
         <v>1</v>
@@ -4179,40 +4196,40 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="23.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="20.25">
       <c r="A2" s="50" t="str">
         <f ca="1">"PHIEÁU THANH TOAÙN LÖÔNG THAÙNG"&amp;TEXT(TODAY()-20," MM-YYYY")</f>
-        <v>PHIEÁU THANH TOAÙN LÖÔNG THAÙNG 04-2022</v>
+        <v>PHIEÁU THANH TOAÙN LÖÔNG THAÙNG 06-2023</v>
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="25"/>
       <c r="D2" s="51" t="str">
         <f ca="1">+A2</f>
-        <v>PHIEÁU THANH TOAÙN LÖÔNG THAÙNG 04-2022</v>
+        <v>PHIEÁU THANH TOAÙN LÖÔNG THAÙNG 06-2023</v>
       </c>
       <c r="E2" s="51"/>
     </row>
-    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="15.75">
       <c r="A3" s="52" t="str">
         <f ca="1">"(PAYSLIP FOR THE MONTH OF "&amp;TRIM(RIGHT(A2,7))&amp;")"</f>
-        <v>(PAYSLIP FOR THE MONTH OF 04-2022)</v>
+        <v>(PAYSLIP FOR THE MONTH OF 06-2023)</v>
       </c>
       <c r="B3" s="52"/>
       <c r="C3" s="25"/>
       <c r="D3" s="53" t="str">
         <f ca="1">A3</f>
-        <v>(PAYSLIP FOR THE MONTH OF 04-2022)</v>
+        <v>(PAYSLIP FOR THE MONTH OF 06-2023)</v>
       </c>
       <c r="E3" s="53"/>
     </row>
-    <row r="4" spans="1:5" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="9.75" customHeight="1">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="25"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" s="26" t="s">
         <v>37</v>
       </c>
@@ -4229,8 +4246,8 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="28" t="s">
+    <row r="6" spans="1:5" ht="21" customHeight="1">
+      <c r="A6" s="26" t="s">
         <v>38</v>
       </c>
       <c r="B6" s="27" t="e">
@@ -4238,7 +4255,7 @@
         <v>#N/A</v>
       </c>
       <c r="C6" s="25"/>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="26" t="s">
         <v>38</v>
       </c>
       <c r="E6" s="27" t="e">
@@ -4246,8 +4263,8 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
+    <row r="7" spans="1:5">
+      <c r="A7" s="26" t="s">
         <v>39</v>
       </c>
       <c r="B7" s="27" t="e">
@@ -4255,7 +4272,7 @@
         <v>#N/A</v>
       </c>
       <c r="C7" s="25"/>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="26" t="s">
         <v>39</v>
       </c>
       <c r="E7" s="27" t="e">
@@ -4263,141 +4280,141 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+    <row r="8" spans="1:5">
+      <c r="A8" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="29" t="e">
+      <c r="B8" s="28" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,5,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C8" s="25"/>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="29" t="e">
+      <c r="E8" s="28" t="e">
         <f>VLOOKUP($E$1,QCChuyen!$A$7:$AI$990,5,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+    <row r="9" spans="1:5">
+      <c r="A9" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="30" t="e">
+      <c r="B9" s="29" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,7,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C9" s="25"/>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="30" t="e">
+      <c r="E9" s="29" t="e">
         <f>VLOOKUP($E$1,QCChuyen!$A$7:$AI$990,7,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
+    <row r="10" spans="1:5" ht="13.5" thickBot="1">
+      <c r="A10" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="30" t="e">
+      <c r="B10" s="29" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,9,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C10" s="25"/>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="30" t="e">
+      <c r="E10" s="29" t="e">
         <f>VLOOKUP($E$1,QCChuyen!$A$7:$AI$990,9,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="5.25" customHeight="1">
       <c r="A11" s="15"/>
       <c r="B11" s="16"/>
       <c r="C11" s="25"/>
       <c r="D11" s="15"/>
       <c r="E11" s="16"/>
     </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="31" t="s">
+    <row r="12" spans="1:5">
+      <c r="A12" s="30" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="21"/>
       <c r="C12" s="25"/>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="30" t="s">
         <v>43</v>
       </c>
       <c r="E12" s="21"/>
     </row>
-    <row r="13" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+    <row r="13" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A13" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="33" t="e">
+      <c r="B13" s="32" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,8,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C13" s="25"/>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="33" t="e">
+      <c r="E13" s="32" t="e">
         <f>VLOOKUP($E$1,QCChuyen!$A$7:$AI$990,8,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="16.5" hidden="1" customHeight="1">
       <c r="A14" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="33"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="25"/>
       <c r="D14" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="33"/>
-    </row>
-    <row r="15" spans="1:5" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="32"/>
+    </row>
+    <row r="15" spans="1:5" ht="16.5" hidden="1" customHeight="1">
       <c r="A15" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="33"/>
+      <c r="B15" s="32"/>
       <c r="C15" s="25"/>
       <c r="D15" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="33"/>
-    </row>
-    <row r="16" spans="1:5" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="32"/>
+    </row>
+    <row r="16" spans="1:5" ht="16.5" hidden="1" customHeight="1">
       <c r="A16" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="25"/>
       <c r="D16" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="33"/>
-    </row>
-    <row r="17" spans="1:5" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="32"/>
+    </row>
+    <row r="17" spans="1:5" ht="16.5" hidden="1" customHeight="1">
       <c r="A17" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="33"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="25"/>
       <c r="D17" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="33"/>
-    </row>
-    <row r="18" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="32"/>
+    </row>
+    <row r="18" spans="1:5" ht="25.5" customHeight="1">
       <c r="A18" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="30" t="e">
+      <c r="B18" s="29" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,10,0)</f>
         <v>#N/A</v>
       </c>
@@ -4405,16 +4422,16 @@
       <c r="D18" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="30" t="e">
+      <c r="E18" s="29" t="e">
         <f>VLOOKUP($E$1,QCChuyen!$A$7:$AI$990,10,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="16.5" customHeight="1">
       <c r="A19" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="30" t="e">
+      <c r="B19" s="29" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,11,0)</f>
         <v>#N/A</v>
       </c>
@@ -4422,55 +4439,55 @@
       <c r="D19" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="E19" s="30" t="e">
+      <c r="E19" s="29" t="e">
         <f>VLOOKUP($E$1,QCChuyen!$A$7:$AI$990,11,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="16.5" hidden="1" customHeight="1">
       <c r="A20" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="34"/>
+      <c r="B20" s="33"/>
       <c r="C20" s="25"/>
       <c r="D20" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="34"/>
-    </row>
-    <row r="21" spans="1:5" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="33"/>
+    </row>
+    <row r="21" spans="1:5" ht="16.5" hidden="1" customHeight="1">
       <c r="A21" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="34"/>
+      <c r="B21" s="33"/>
       <c r="C21" s="25"/>
       <c r="D21" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="34"/>
-    </row>
-    <row r="22" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
+      <c r="E21" s="33"/>
+    </row>
+    <row r="22" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A22" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="35" t="e">
+      <c r="B22" s="34" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,12,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C22" s="25"/>
-      <c r="D22" s="32" t="s">
+      <c r="D22" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="35" t="e">
+      <c r="E22" s="34" t="e">
         <f>VLOOKUP($E$1,QCChuyen!$A$7:$AI$990,12,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="16.5" customHeight="1">
       <c r="A23" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="30" t="e">
+      <c r="B23" s="29" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,13,0)</f>
         <v>#N/A</v>
       </c>
@@ -4478,72 +4495,72 @@
       <c r="D23" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="30" t="e">
+      <c r="E23" s="29" t="e">
         <f>VLOOKUP($E$1,QCChuyen!$A$7:$AI$990,13,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
+    <row r="24" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A24" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="30" t="e">
+      <c r="B24" s="29" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,14,0)+VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,16,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C24" s="25"/>
-      <c r="D24" s="32" t="s">
+      <c r="D24" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="30" t="e">
+      <c r="E24" s="29" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,14,0)+VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,16,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="32" t="s">
+    <row r="25" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A25" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="30" t="e">
+      <c r="B25" s="29" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,15,0)+VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,17,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C25" s="25"/>
-      <c r="D25" s="32" t="s">
+      <c r="D25" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="E25" s="30" t="e">
+      <c r="E25" s="29" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,15,0)+VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,17,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="16.5" hidden="1" customHeight="1">
       <c r="A26" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="33"/>
+      <c r="B26" s="32"/>
       <c r="C26" s="25"/>
       <c r="D26" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="33"/>
-    </row>
-    <row r="27" spans="1:5" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="32"/>
+    </row>
+    <row r="27" spans="1:5" ht="16.5" hidden="1" customHeight="1">
       <c r="A27" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="34"/>
+      <c r="B27" s="33"/>
       <c r="C27" s="25"/>
       <c r="D27" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="34"/>
-    </row>
-    <row r="28" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="33"/>
+    </row>
+    <row r="28" spans="1:5" ht="16.5" customHeight="1">
       <c r="A28" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="30" t="e">
+      <c r="B28" s="29" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,21,0)</f>
         <v>#N/A</v>
       </c>
@@ -4551,16 +4568,16 @@
       <c r="D28" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="E28" s="30" t="e">
+      <c r="E28" s="29" t="e">
         <f>VLOOKUP($E$1,QCChuyen!$A$7:$AI$990,21,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="16.5" customHeight="1">
       <c r="A29" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B29" s="30" t="e">
+      <c r="B29" s="29" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,22,0)</f>
         <v>#N/A</v>
       </c>
@@ -4568,16 +4585,16 @@
       <c r="D29" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="E29" s="30" t="e">
+      <c r="E29" s="29" t="e">
         <f>VLOOKUP($E$1,QCChuyen!$A$7:$AI$990,22,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="16.5" customHeight="1">
       <c r="A30" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B30" s="30" t="e">
+      <c r="B30" s="29" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,23,0)</f>
         <v>#N/A</v>
       </c>
@@ -4585,16 +4602,16 @@
       <c r="D30" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E30" s="30" t="e">
+      <c r="E30" s="29" t="e">
         <f>VLOOKUP($E$1,QCChuyen!$A$7:$AI$990,23,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="16.5" customHeight="1">
       <c r="A31" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="30" t="e">
+      <c r="B31" s="29" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,25,0)</f>
         <v>#N/A</v>
       </c>
@@ -4602,16 +4619,16 @@
       <c r="D31" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="E31" s="30" t="e">
+      <c r="E31" s="29" t="e">
         <f>VLOOKUP($E$1,QCChuyen!$A$7:$AI$990,25,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="16.5" customHeight="1">
       <c r="A32" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="B32" s="30" t="e">
+      <c r="B32" s="29" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,24,0)</f>
         <v>#N/A</v>
       </c>
@@ -4619,16 +4636,16 @@
       <c r="D32" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="E32" s="30" t="e">
+      <c r="E32" s="29" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,24,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="16.5" customHeight="1">
       <c r="A33" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="30" t="e">
+      <c r="B33" s="29" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,26,0)</f>
         <v>#N/A</v>
       </c>
@@ -4636,16 +4653,16 @@
       <c r="D33" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="E33" s="30" t="e">
+      <c r="E33" s="29" t="e">
         <f>VLOOKUP($E$1,QCChuyen!$A$7:$AI$990,26,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="B34" s="30" t="e">
+      <c r="B34" s="29" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AL$990,37,0)</f>
         <v>#N/A</v>
       </c>
@@ -4653,16 +4670,16 @@
       <c r="D34" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="E34" s="30" t="e">
+      <c r="E34" s="29" t="e">
         <f>VLOOKUP($E$1,QCChuyen!$A$7:$AL$990,37,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B35" s="30" t="e">
+      <c r="B35" s="29" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AL$990,38,0)</f>
         <v>#N/A</v>
       </c>
@@ -4670,13 +4687,13 @@
       <c r="D35" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="E35" s="30" t="e">
+      <c r="E35" s="29" t="e">
         <f>VLOOKUP($E$1,QCChuyen!$A$7:$AL$990,38,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="36" t="s">
+    <row r="36" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A36" s="35" t="s">
         <v>57</v>
       </c>
       <c r="B36" s="20" t="e">
@@ -4684,7 +4701,7 @@
         <v>#N/A</v>
       </c>
       <c r="C36" s="25"/>
-      <c r="D36" s="36" t="s">
+      <c r="D36" s="35" t="s">
         <v>57</v>
       </c>
       <c r="E36" s="20" t="e">
@@ -4692,46 +4709,46 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="6" customHeight="1">
       <c r="A37" s="17"/>
-      <c r="B37" s="37" t="e">
+      <c r="B37" s="36" t="e">
         <f>IF(+B18+B19+B22+B23+B26+B27+ROUND(SUM(B28:B33),0)=B36-1,"","Sai")</f>
         <v>#N/A</v>
       </c>
-      <c r="C37" s="38"/>
+      <c r="C37" s="37"/>
       <c r="D37" s="17"/>
-      <c r="E37" s="37" t="e">
+      <c r="E37" s="36" t="e">
         <f>IF(+E18+E19+E22+E23+E26+E27+ROUND(SUM(E28:E33),0)=E36-1,"","Sai")</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="31" t="s">
+    <row r="38" spans="1:5" ht="17.25" customHeight="1">
+      <c r="A38" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="39"/>
+      <c r="B38" s="38"/>
       <c r="C38" s="25"/>
-      <c r="D38" s="31" t="s">
+      <c r="D38" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="E38" s="39"/>
-    </row>
-    <row r="39" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="32" t="s">
+      <c r="E38" s="38"/>
+    </row>
+    <row r="39" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A39" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="B39" s="34"/>
+      <c r="B39" s="33"/>
       <c r="C39" s="25"/>
-      <c r="D39" s="32" t="s">
+      <c r="D39" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="E39" s="34"/>
-    </row>
-    <row r="40" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E39" s="33"/>
+    </row>
+    <row r="40" spans="1:5" ht="16.5" customHeight="1">
       <c r="A40" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="34" t="e">
+      <c r="B40" s="33" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,29,0)</f>
         <v>#N/A</v>
       </c>
@@ -4739,81 +4756,81 @@
       <c r="D40" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="E40" s="34" t="e">
+      <c r="E40" s="33" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,29,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="32" t="s">
+    <row r="41" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A41" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="B41" s="34" t="e">
+      <c r="B41" s="33" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,28,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C41" s="25"/>
-      <c r="D41" s="32" t="s">
+      <c r="D41" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="E41" s="34" t="e">
+      <c r="E41" s="33" t="e">
         <f>VLOOKUP($E$1,QCChuyen!$A$7:$AI$990,28,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="32" t="s">
+    <row r="42" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A42" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="34" t="e">
+      <c r="B42" s="33" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,31,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C42" s="25"/>
-      <c r="D42" s="32" t="s">
+      <c r="D42" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="E42" s="34" t="e">
+      <c r="E42" s="33" t="e">
         <f>VLOOKUP($E$1,QCChuyen!$A$7:$AI$990,31,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="32" t="s">
+    <row r="43" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A43" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B43" s="34" t="e">
+      <c r="B43" s="33" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,30,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C43" s="25"/>
-      <c r="D43" s="32" t="s">
+      <c r="D43" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="E43" s="34" t="e">
+      <c r="E43" s="33" t="e">
         <f>VLOOKUP($E$1,QCChuyen!$A$7:$AI$990,30,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="32" t="s">
+    <row r="44" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A44" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="B44" s="34" t="e">
+      <c r="B44" s="33" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,32,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C44" s="25"/>
-      <c r="D44" s="32" t="s">
+      <c r="D44" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="E44" s="34" t="e">
+      <c r="E44" s="33" t="e">
         <f>VLOOKUP($E$1,QCChuyen!$A$7:$AI$990,32,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="40" t="s">
+    <row r="45" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A45" s="39" t="s">
         <v>65</v>
       </c>
       <c r="B45" s="20" t="e">
@@ -4821,7 +4838,7 @@
         <v>#N/A</v>
       </c>
       <c r="C45" s="25"/>
-      <c r="D45" s="40" t="s">
+      <c r="D45" s="39" t="s">
         <v>65</v>
       </c>
       <c r="E45" s="20" t="e">
@@ -4829,48 +4846,48 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="41" t="str">
+    <row r="46" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A46" s="40" t="str">
         <f>"Ghi chuù (Note): "&amp;IF(ISNA(VLOOKUP(RIGHT(B5,4),'[1]Ghi chu dieu chinh'!$B$8:$AL$302,33,0)),"",VLOOKUP(RIGHT(B5,4),'[1]Ghi chu dieu chinh'!$B$8:$AL$302,33,0))</f>
         <v xml:space="preserve">Ghi chuù (Note): </v>
       </c>
       <c r="B46" s="20"/>
       <c r="C46" s="25"/>
-      <c r="D46" s="41" t="str">
+      <c r="D46" s="40" t="str">
         <f>"Ghi chuù (Note): "&amp;IF(ISNA(VLOOKUP(RIGHT(E5,4),'[1]Ghi chu dieu chinh'!$B$8:$AL$302,33,0)),"",VLOOKUP(RIGHT(E5,4),'[1]Ghi chu dieu chinh'!$B$8:$AL$302,33,0))</f>
         <v xml:space="preserve">Ghi chuù (Note): </v>
       </c>
       <c r="E46" s="20"/>
     </row>
-    <row r="47" spans="1:5" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="3.75" customHeight="1">
       <c r="A47" s="19"/>
-      <c r="B47" s="42"/>
-      <c r="C47" s="43"/>
+      <c r="B47" s="41"/>
+      <c r="C47" s="42"/>
       <c r="D47" s="18"/>
-      <c r="E47" s="42"/>
-    </row>
-    <row r="48" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E47" s="41"/>
+    </row>
+    <row r="48" spans="1:5" ht="18.75" customHeight="1">
       <c r="A48" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B48" s="44" t="e">
+      <c r="B48" s="43" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,34,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="C48" s="45"/>
+      <c r="C48" s="44"/>
       <c r="D48" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E48" s="44" t="e">
+      <c r="E48" s="43" t="e">
         <f>VLOOKUP($E$1,QCChuyen!$A$7:$AI$990,34,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="20.25" customHeight="1">
       <c r="A49" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="B49" s="44" t="e">
+      <c r="B49" s="43" t="e">
         <f>VLOOKUP($B$1,QCChuyen!$A$7:$AI$990,35,0)</f>
         <v>#N/A</v>
       </c>
@@ -4878,19 +4895,19 @@
       <c r="D49" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="E49" s="44" t="e">
+      <c r="E49" s="43" t="e">
         <f>VLOOKUP($E$1,QCChuyen!$A$7:$AI$990,35,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="6.75" customHeight="1">
       <c r="A50" s="21"/>
       <c r="B50" s="22"/>
       <c r="C50" s="25"/>
       <c r="D50" s="21"/>
       <c r="E50" s="22"/>
     </row>
-    <row r="51" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="17.25" customHeight="1">
       <c r="A51" s="23" t="s">
         <v>66</v>
       </c>
@@ -4901,56 +4918,56 @@
       </c>
       <c r="E51" s="24"/>
     </row>
-    <row r="52" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="5.25" customHeight="1">
       <c r="A52" s="23"/>
       <c r="B52" s="24"/>
       <c r="C52" s="25"/>
       <c r="D52" s="23"/>
       <c r="E52" s="24"/>
     </row>
-    <row r="53" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="46" t="s">
+    <row r="53" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A53" s="45" t="s">
         <v>67</v>
       </c>
       <c r="B53" s="24"/>
       <c r="C53" s="25"/>
-      <c r="D53" s="46" t="s">
+      <c r="D53" s="45" t="s">
         <v>67</v>
       </c>
       <c r="E53" s="24"/>
     </row>
-    <row r="54" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="46" t="s">
+    <row r="54" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A54" s="45" t="s">
         <v>68</v>
       </c>
       <c r="B54" s="24"/>
       <c r="C54" s="25"/>
-      <c r="D54" s="46" t="s">
+      <c r="D54" s="45" t="s">
         <v>68</v>
       </c>
       <c r="E54" s="24"/>
     </row>
-    <row r="55" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="46" t="s">
+    <row r="55" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A55" s="45" t="s">
         <v>69</v>
       </c>
       <c r="B55" s="24"/>
       <c r="C55" s="25"/>
-      <c r="D55" s="46" t="s">
+      <c r="D55" s="45" t="s">
         <v>69</v>
       </c>
       <c r="E55" s="24"/>
     </row>
-    <row r="56" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="46" t="s">
+    <row r="56" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A56" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="B56" s="46"/>
-      <c r="C56" s="47"/>
-      <c r="D56" s="46" t="s">
+      <c r="B56" s="45"/>
+      <c r="C56" s="46"/>
+      <c r="D56" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="E56" s="46"/>
+      <c r="E56" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4969,12 +4986,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData/>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>